<commit_message>
feb 24 slides and lab 2 deflections
</commit_message>
<xml_diff>
--- a/activities/lab2_deflections.xlsx
+++ b/activities/lab2_deflections.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emilymaloney/Dropbox/Grad_School/soc490s/activities/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{939A9246-DC7B-F542-AD39-9F41C965CAA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFFBC5DA-A66A-F14C-8A89-8486C267132E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16280" xr2:uid="{8739246B-3B30-E943-92FA-C772922BD23E}"/>
   </bookViews>
@@ -640,7 +640,7 @@
   <dimension ref="A1:D57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -670,248 +670,248 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D2" s="1">
-        <v>7.2</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
+      <c r="C3" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="D3" s="1">
-        <v>2.7</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="D4" s="1">
-        <v>3.2</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="D5" s="1">
-        <v>4.8</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="D6" s="1">
-        <v>4.3</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="D7" s="1">
-        <v>1.2</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="1">
-        <v>6</v>
+        <v>6</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1.3</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>15</v>
+        <v>6</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>29</v>
       </c>
       <c r="D9" s="1">
-        <v>0.9</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>16</v>
+        <v>6</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="D10" s="1">
-        <v>2.4</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="D11" s="1">
-        <v>1.8</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>18</v>
+        <v>6</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="D12" s="1">
-        <v>2.1</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="4">
-        <v>1.3</v>
+        <v>6</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="1">
+        <v>5.5</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>20</v>
+        <v>6</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="D14" s="1">
-        <v>7.5</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>21</v>
+      <c r="C15" s="12" t="s">
+        <v>55</v>
       </c>
       <c r="D15" s="1">
-        <v>8.5</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>22</v>
+      <c r="C16" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="D16" s="1">
-        <v>4.0999999999999996</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="D17" s="1">
-        <v>6.2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>24</v>
+        <v>8</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="D18" s="1">
-        <v>4.5999999999999996</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>25</v>
+        <v>8</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="D19" s="1">
         <v>4.0999999999999996</v>
@@ -933,254 +933,254 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>27</v>
+        <v>8</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="D21" s="1">
-        <v>1.6</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>28</v>
+        <v>8</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="D22" s="1">
-        <v>2.1</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>29</v>
+        <v>8</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>30</v>
       </c>
       <c r="D23" s="1">
-        <v>2.1</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>30</v>
+      <c r="C24" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="D24" s="1">
-        <v>5.4</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>31</v>
+        <v>8</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="D25" s="1">
-        <v>2.8</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>32</v>
+        <v>8</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="D26" s="1">
-        <v>9.9</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D27" s="3">
-        <v>1.3</v>
+        <v>50</v>
+      </c>
+      <c r="D27" s="1">
+        <v>3.2</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>34</v>
+      <c r="C28" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="D28" s="1">
-        <v>7.9</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>35</v>
+        <v>8</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>56</v>
       </c>
       <c r="D29" s="1">
-        <v>5.5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>28</v>
+        <v>10</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D30" s="1">
-        <v>2.1</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>29</v>
+        <v>10</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="D31" s="1">
-        <v>2.1</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D32" s="1">
-        <v>5.4</v>
+        <v>10</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D32" s="4">
+        <v>1.3</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C33" s="10" t="s">
-        <v>31</v>
+      <c r="C33" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="D33" s="1">
-        <v>2.8</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>36</v>
+        <v>10</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>27</v>
       </c>
       <c r="D34" s="1">
-        <v>5.2</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>37</v>
+        <v>10</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="D35" s="1">
-        <v>5.4</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>38</v>
+        <v>10</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="D36" s="1">
-        <v>5.9</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C37" s="4" t="s">
-        <v>39</v>
+      <c r="C37" s="10" t="s">
+        <v>31</v>
       </c>
       <c r="D37" s="1">
-        <v>1.5</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>40</v>
+        <v>10</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="D38" s="1">
-        <v>12.5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -1188,10 +1188,10 @@
         <v>10</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>41</v>
+        <v>10</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="D39" s="1">
         <v>3.4</v>
@@ -1199,240 +1199,240 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="D40" s="1">
-        <v>4.5</v>
+        <v>8.3000000000000007</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="D41" s="1">
-        <v>3.4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>44</v>
+        <v>10</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="D42" s="1">
-        <v>1.4</v>
+        <v>8.3000000000000007</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>45</v>
+        <v>10</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>57</v>
       </c>
       <c r="D43" s="1">
-        <v>1.8</v>
+        <v>9.1</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>46</v>
+        <v>4</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="D44" s="1">
-        <v>3.1</v>
+        <v>7.2</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>47</v>
+        <v>4</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D45" s="1">
-        <v>8.3000000000000007</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C46" s="2" t="s">
-        <v>48</v>
+      <c r="C46" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="D46" s="1">
-        <v>11.1</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>49</v>
+        <v>4</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="D47" s="1">
-        <v>5.5</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>50</v>
+        <v>4</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="D48" s="1">
-        <v>3.2</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>51</v>
+        <v>4</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="D49" s="1">
-        <v>8</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="D50" s="1">
-        <v>1.4</v>
+        <v>9.9</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>53</v>
+        <v>4</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>28</v>
       </c>
       <c r="D51" s="1">
-        <v>1.8</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>46</v>
+        <v>4</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>36</v>
       </c>
       <c r="D52" s="1">
-        <v>3.1</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>47</v>
+        <v>4</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>40</v>
       </c>
       <c r="D53" s="1">
-        <v>8.3000000000000007</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C54" s="11" t="s">
-        <v>54</v>
+      <c r="C54" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="D54" s="1">
-        <v>11.2</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C55" s="12" t="s">
-        <v>55</v>
+        <v>4</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="D55" s="1">
-        <v>10.6</v>
+        <v>11.1</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C56" s="12" t="s">
-        <v>56</v>
+        <v>4</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>52</v>
       </c>
       <c r="D56" s="1">
-        <v>6</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
@@ -1440,16 +1440,19 @@
         <v>14</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C57" s="12" t="s">
-        <v>57</v>
+        <v>4</v>
+      </c>
+      <c r="C57" s="11" t="s">
+        <v>54</v>
       </c>
       <c r="D57" s="1">
-        <v>9.1</v>
+        <v>11.2</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D57">
+    <sortCondition ref="B2:B57"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>